<commit_message>
took avg over runs
</commit_message>
<xml_diff>
--- a/data/inputs/test.xlsx
+++ b/data/inputs/test.xlsx
@@ -461,10 +461,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T10" activeCellId="0" sqref="T10"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
@@ -491,13 +491,13 @@
     </row>
     <row r="2" ht="16.5" customHeight="1" s="4">
       <c r="A2" s="3" t="n">
-        <v>11</v>
+        <v>-5</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1" s="4">
@@ -508,28 +508,61 @@
         <v>3</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1" s="4">
       <c r="A4" s="3" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1" s="4">
       <c r="A5" s="3" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>3</v>
       </c>
       <c r="C5" s="3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="4">
+      <c r="A6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="4">
+      <c r="A7" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" ht="15" customHeight="1" s="4">
+      <c r="A8" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="3" t="n">
         <v>7</v>
       </c>
     </row>

</xml_diff>